<commit_message>
modifications to test plan
</commit_message>
<xml_diff>
--- a/SchubertPeter_p2_test_plan.xlsx
+++ b/SchubertPeter_p2_test_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterschubert/Peter_Documents/University of Michigan-Dearborn/CIS 435/schubertPeter_cis435_p2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B97F09-8A6B-CE45-8A39-A98633228F7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A199FFA5-F333-6243-90A6-F0BB7F7B618F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="28800" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="October 23, 2020" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="50">
   <si>
     <t>Test case plan</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>When a player clicks on a cell, the paragraph element below the grid changes the turn of each player (either X or O)</t>
+  </si>
+  <si>
+    <t>The page loads the appropriate background color and shadow to the elements and page</t>
   </si>
 </sst>
 </file>
@@ -677,8 +680,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1149,7 +1152,472 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="35.5" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>44128</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="86" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="4" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27720113-11A3-E348-A4C7-88D867B82C2D}">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -1181,471 +1649,6 @@
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
-        <v>44128</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <v>7</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>8</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>9</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>10</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>12</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>13</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27720113-11A3-E348-A4C7-88D867B82C2D}">
-  <dimension ref="A1:I19"/>
-  <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" customWidth="1"/>
-    <col min="4" max="4" width="35.5" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" customWidth="1"/>
-    <col min="6" max="6" width="19.5" customWidth="1"/>
-    <col min="7" max="7" width="16.5" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-    </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
         <v>44129</v>
       </c>
       <c r="B2" s="10"/>

</xml_diff>